<commit_message>
Add lines between cells
</commit_message>
<xml_diff>
--- a/WHS- Potential Data.xlsx
+++ b/WHS- Potential Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerstinwolf/DS Projects/GitHub/World_Health_Statistics_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B08FB26-7FDF-C140-8B43-BB83657CA23B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7009D2C7-5722-0B4F-A91C-67F39DCE2D2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3020" yWindow="3140" windowWidth="24840" windowHeight="17440" xr2:uid="{73079E3D-8FAF-AF49-B9BF-803FC402AFAB}"/>
   </bookViews>
@@ -395,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -429,30 +429,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -771,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDE3DD7-2B58-7B4B-82FB-5A16291656B6}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,417 +816,417 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="4" t="s">
         <v>41</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" ht="340" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:23" s="6" customFormat="1" ht="340" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="6">
         <v>2000</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="2">
         <v>2006</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>2009</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="8" t="s">
         <v>31</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="6">
         <v>2008</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="6">
         <v>2013</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="2">
         <v>2004</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="3" customFormat="1" ht="136" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:23" s="6" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="6">
         <v>2002</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>2010</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <v>2010</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="2">
         <v>2004</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="6">
         <v>2000</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="6">
         <v>2009</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="6">
         <v>2014</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="2">
         <v>2009</v>
       </c>
-      <c r="W3" s="3">
+      <c r="W3" s="6">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="4" spans="1:23" s="6" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <v>2014</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <v>2008</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="6">
         <v>2010</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="6">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="5" spans="1:23" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <v>2005</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>2006</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="2">
         <v>2007</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="2">
         <v>2010</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="6">
         <v>2004</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="6">
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="6" spans="1:23" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>2004</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>2005</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>2017</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <v>2012</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6" s="6">
         <v>2009</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:23" s="6" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
         <v>2007</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>2001</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
         <v>2009</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="6">
         <v>2012</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="T7" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="8" spans="1:23" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>2001</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <v>2000</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="6">
         <v>2016</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="6">
         <v>2010</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="9" spans="1:23" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>2011</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>2000</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q9" s="2"/>
-      <c r="T9" s="3">
+      <c r="Q9" s="8"/>
+      <c r="T9" s="6">
         <v>2008</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="10" spans="1:23" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="6">
         <v>2015</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10" s="6">
         <v>2011</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="11" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <v>2014</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T11" s="6">
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="12" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <v>2012</v>
       </c>
-      <c r="T12" s="3">
+      <c r="T12" s="6">
         <v>2007</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="13" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="6">
         <v>2016</v>
       </c>
-      <c r="T13" s="3">
+      <c r="T13" s="6">
         <v>2006</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="14" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="15" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="16" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
     </row>

</xml_diff>